<commit_message>
test(results.xlsx): add user studies 2 results
</commit_message>
<xml_diff>
--- a/_usertests/Results.xlsx
+++ b/_usertests/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="39300" yWindow="-4420" windowWidth="12800" windowHeight="20020" tabRatio="500"/>
+    <workbookView xWindow="39300" yWindow="-4420" windowWidth="12800" windowHeight="20020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Nina User1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="116">
   <si>
     <t>User 1</t>
   </si>
@@ -319,6 +319,57 @@
   </si>
   <si>
     <t>Correctness</t>
+  </si>
+  <si>
+    <t>Lady Gaga</t>
+  </si>
+  <si>
+    <t>Prince of England, Marriage</t>
+  </si>
+  <si>
+    <t>Two Grizzly bears</t>
+  </si>
+  <si>
+    <t>Gumball machine</t>
+  </si>
+  <si>
+    <t>The painting, with the pitchfork</t>
+  </si>
+  <si>
+    <t>Yoga, outside in the mountains</t>
+  </si>
+  <si>
+    <t>Some white dude cooking</t>
+  </si>
+  <si>
+    <t>Starship</t>
+  </si>
+  <si>
+    <t>Dragon, fire</t>
+  </si>
+  <si>
+    <t>Eggrolls</t>
+  </si>
+  <si>
+    <t>Horse racing</t>
+  </si>
+  <si>
+    <t>Clocks, doorway</t>
+  </si>
+  <si>
+    <t>Family doing kissy faces</t>
+  </si>
+  <si>
+    <t>Graduation</t>
+  </si>
+  <si>
+    <t>Nina and Molly sleeping</t>
+  </si>
+  <si>
+    <t>Happy and Molly</t>
+  </si>
+  <si>
+    <t>Person in the bottom right, storefronts</t>
   </si>
 </sst>
 </file>
@@ -379,8 +430,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -395,13 +452,19 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -733,7 +796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -954,15 +1017,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -970,108 +1033,175 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="B10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>66</v>
       </c>
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>